<commit_message>
fixed date formats (start_date_ymd and end_date_ymd)
</commit_message>
<xml_diff>
--- a/database/data_to_add/added/2020-02-05jeff/clariidae_ayinla_1988.xlsx
+++ b/database/data_to_add/added/2020-02-05jeff/clariidae_ayinla_1988.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff.Wesner\Documents\GitHub\Freshwater-Fish-Diet-Database\database\data_to_add\2020-01-25jeff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff.Wesner\Documents\GitHub\Freshwater-Fish-Diet-Database\database\data_to_add\added\2020-02-05jeff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A99C1D6-BA80-4580-8786-BA2F491DFB7A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B13C28-34B0-4F57-8C86-1DC16BEB3BC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{489F0415-0AB9-412C-9822-F74D0E3629D1}"/>
   </bookViews>
@@ -603,12 +603,12 @@
   <dimension ref="A1:AR4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AR4" sqref="AR4"/>
+      <selection activeCell="AO1" sqref="AO1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -742,7 +742,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -864,7 +864,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -986,7 +986,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>45</v>
       </c>

</xml_diff>